<commit_message>
Drop downs and validation errors
</commit_message>
<xml_diff>
--- a/Project overview.xlsx
+++ b/Project overview.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>Important</t>
   </si>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t>5th Jan</t>
+  </si>
+  <si>
+    <t>7th Jan</t>
+  </si>
+  <si>
+    <t>Changed Backend Architecture from ajax to URL variables to include dropdowns</t>
+  </si>
+  <si>
+    <t>Added php backend and modified query for "I want to buy a home"option</t>
+  </si>
+  <si>
+    <t>Updated javascript validation errors</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1358,6 +1370,27 @@
         <v>84</v>
       </c>
     </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hours and dropdown work
</commit_message>
<xml_diff>
--- a/Project overview.xlsx
+++ b/Project overview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16440" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="100">
   <si>
     <t>Important</t>
   </si>
@@ -303,6 +303,36 @@
   </si>
   <si>
     <t>Updated javascript validation errors</t>
+  </si>
+  <si>
+    <t>Dropdowns</t>
+  </si>
+  <si>
+    <t>bank description</t>
+  </si>
+  <si>
+    <t>remove features to keep only 3</t>
+  </si>
+  <si>
+    <t>9th Jan</t>
+  </si>
+  <si>
+    <t>Updated dynamic dropdowns for:</t>
+  </si>
+  <si>
+    <t>Refinance/buy new</t>
+  </si>
+  <si>
+    <t>owner/investor</t>
+  </si>
+  <si>
+    <t>principal&amp;interest/interest</t>
+  </si>
+  <si>
+    <t>offset/redraw</t>
+  </si>
+  <si>
+    <t>updated javascript function to show hide dropdowns</t>
   </si>
 </sst>
 </file>
@@ -312,7 +342,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +356,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -364,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -382,6 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,10 +925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R20"/>
+  <dimension ref="B2:R26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1112,6 +1150,21 @@
       </c>
       <c r="C20" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1273,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1391,6 +1444,42 @@
         <v>89</v>
       </c>
     </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Product login and sql change
</commit_message>
<xml_diff>
--- a/Project overview.xlsx
+++ b/Project overview.xlsx
@@ -416,10 +416,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,7 +1085,7 @@
       <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1093,7 +1093,7 @@
       <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
@@ -1131,7 +1131,7 @@
       <c r="B18" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D18" t="s">
@@ -1142,7 +1142,7 @@
       <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
@@ -1456,27 +1456,27 @@
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified tables according to Ratecity
</commit_message>
<xml_diff>
--- a/Project overview.xlsx
+++ b/Project overview.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="125">
   <si>
     <t>Important</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>Rate City scrape script</t>
+  </si>
+  <si>
+    <t>9th Feb</t>
+  </si>
+  <si>
+    <t>SQL script: JSON to csv and Insert statements</t>
+  </si>
+  <si>
+    <t>Data extraction from SQL (shell script)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +417,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,10 +434,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -467,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -482,11 +499,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1152,7 +1171,7 @@
       <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1160,7 +1179,7 @@
       <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
@@ -1198,7 +1217,7 @@
       <c r="B18" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D18" t="s">
@@ -1209,7 +1228,7 @@
       <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
@@ -1393,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D36"/>
+  <dimension ref="B2:D38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1405,274 +1424,328 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="12">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="B6" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="12">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="B7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="B8" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="12">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="B11" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="12">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="B12" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="12">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="B15" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="12">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D16" s="10" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="10" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="10" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="10" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="10" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="B21" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="12">
         <v>10</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="11" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="11" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="B24" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="12">
         <v>2</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="B25" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="12">
         <v>9</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="11" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D27" s="11" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="11" t="s">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+      <c r="B29" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="12">
         <v>5</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="11" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="11" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="11" t="s">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+      <c r="B33" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="12">
         <v>8</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="12" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="B34" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="12">
         <v>7</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="12" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+      <c r="B35" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="12">
         <v>1</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="12" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="B36" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="12">
         <v>8</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="12" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="10">
+        <v>8</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mobile views and colour changes
</commit_message>
<xml_diff>
--- a/Project overview.xlsx
+++ b/Project overview.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="190">
   <si>
     <t>Important</t>
   </si>
@@ -592,6 +592,18 @@
   </si>
   <si>
     <t>Header changes, 3 icons, colour changes, buttons/hover</t>
+  </si>
+  <si>
+    <t>25th Feb</t>
+  </si>
+  <si>
+    <t>Search page fonts, changing logo, resizing index and search page icons.</t>
+  </si>
+  <si>
+    <t>Mobile views</t>
+  </si>
+  <si>
+    <t>javascript logic (limit max value for loan)</t>
   </si>
 </sst>
 </file>
@@ -1778,10 +1790,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E69"/>
+  <dimension ref="B1:E74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2394,6 +2406,43 @@
         <v>185</v>
       </c>
     </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>186</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D72" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D73" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D74" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>